<commit_message>
Add notes to calculations
</commit_message>
<xml_diff>
--- a/specs/patch_antenna-calculations.xlsx
+++ b/specs/patch_antenna-calculations.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
   <si>
     <t>Ground (mm)</t>
   </si>
@@ -120,6 +120,15 @@
   </si>
   <si>
     <t>Note: Width and length are swapped from reference paper.</t>
+  </si>
+  <si>
+    <t>Notes:</t>
+  </si>
+  <si>
+    <t>Ground plane occupies the entire bottom layer.</t>
+  </si>
+  <si>
+    <t>Feed position starts its origin coordinates from the bottom left corner of the patch.</t>
   </si>
 </sst>
 </file>
@@ -455,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -885,6 +894,19 @@
         <v>0</v>
       </c>
     </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Cleanup layout, files, and calculations
</commit_message>
<xml_diff>
--- a/specs/patch_antenna-calculations.xlsx
+++ b/specs/patch_antenna-calculations.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jzheng13\Documents\HA-HA\specs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeffrey Zheng\Dropbox\HA-HA\specs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
   <si>
     <t>Ground (mm)</t>
   </si>
@@ -77,9 +77,6 @@
     <t>+/-0.02</t>
   </si>
   <si>
-    <t>Dielectric Constant (eff)</t>
-  </si>
-  <si>
     <t>Reference</t>
   </si>
   <si>
@@ -125,17 +122,29 @@
     <t>Notes:</t>
   </si>
   <si>
-    <t>Ground plane occupies the entire bottom layer.</t>
-  </si>
-  <si>
     <t>Feed position starts its origin coordinates from the bottom left corner of the patch.</t>
+  </si>
+  <si>
+    <t>Dielectric Constant (Effective)</t>
+  </si>
+  <si>
+    <t>Ground plane and substrate continues to occupy the rest of the bottom layer.</t>
+  </si>
+  <si>
+    <t>Transmission line impedance of 49.9ohms achieved with 104mil width.</t>
+  </si>
+  <si>
+    <t>of effective wavelength</t>
+  </si>
+  <si>
+    <t>Effecitve dielectric constant of reference design is 3.86.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,6 +167,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -176,16 +193,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -199,6 +220,61 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>505302</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>105082</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41B45DFE-EEAD-43E9-9429-14F36F1778A4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11925300" y="2286000"/>
+          <a:ext cx="3419952" cy="2200582"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -464,451 +540,517 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <v>4.58</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="3">
+        <f>(B3+1)/2+(B3-1)/2*((SQRT(1+12*B6/G14))^-1)</f>
+        <v>4.2728372472104468</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1.9</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="3">
+        <v>2.4500000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="3">
+        <f>300000000/(B7*10^6)/SQRT(B4)</f>
+        <v>59.237537269949385</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="3">
+        <f>B8*0.0393701*1000</f>
+        <v>2332.1877660716345</v>
+      </c>
+      <c r="C9" s="3">
+        <f>B9/2</f>
+        <v>1166.0938830358173</v>
+      </c>
+      <c r="D9" s="3">
+        <f>B9/4</f>
+        <v>583.04694151790864</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B4">
-        <f>(B3+1)/2+(B3-1)/2*((SQRT(1+12*B5/E14))^-1)</f>
-        <v>4.3194951107791084</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6">
-        <v>2.4500000000000002</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7">
-        <f>300000000/(B6*10^6)/SQRT(B4)</f>
-        <v>58.916735748293618</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8">
-        <f>B7*0.0393701*1000</f>
-        <v>2319.5577780838944</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9">
-        <v>1.9</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="B11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11"/>
-      <c r="D11"/>
-      <c r="E11"/>
-      <c r="F11"/>
-      <c r="G11"/>
-      <c r="H11"/>
-      <c r="I11"/>
-      <c r="K11" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
+      <c r="K11" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="I12" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="3">
         <v>42</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="3">
         <f>B13*0.0393701*1000</f>
         <v>1653.5442</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="3">
         <v>42</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="3">
         <f>D13*0.0393701*1000</f>
         <v>1653.5442</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="3">
         <v>33</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="3">
         <f>F13*0.0393701*1000</f>
         <v>1299.2132999999999</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="3">
         <v>13</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="3">
         <f>H13*0.0393701*1000</f>
         <v>511.81129999999996</v>
       </c>
+      <c r="J13" s="1">
+        <f>G13/B9</f>
+        <v>0.55707920215549822</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="3">
         <v>47</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="3">
         <f t="shared" ref="C14:E15" si="0">B14*0.0393701*1000</f>
         <v>1850.3946999999998</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="3">
         <v>47</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="3">
         <f t="shared" si="0"/>
         <v>1850.3946999999998</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="3">
         <v>38</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="3">
         <f t="shared" ref="G14" si="1">F14*0.0393701*1000</f>
         <v>1496.0637999999999</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="3">
         <v>3</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="3">
         <f t="shared" ref="I14" si="2">H14*0.0393701*1000</f>
         <v>118.1103</v>
       </c>
+      <c r="J14" s="1">
+        <f>G14/B9</f>
+        <v>0.64148514187602823</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="2">
         <v>0.2</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="2">
         <f t="shared" si="0"/>
         <v>7.8740200000000007</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="3">
         <v>1.5</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="3">
         <f t="shared" si="0"/>
         <v>59.055149999999998</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="3">
         <v>0.02</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="3">
         <f t="shared" ref="G15" si="3">F15*0.0393701*1000</f>
         <v>0.78740199999999994</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="3">
         <v>0.02</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="3">
         <f t="shared" ref="I15" si="4">H15*0.0393701*1000</f>
         <v>0.78740199999999994</v>
       </c>
     </row>
-    <row r="17" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="3"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J26" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="2" t="s">
+      <c r="K26" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" s="3">
+        <f>C27/0.0393701/1000</f>
+        <v>41.909977368612218</v>
+      </c>
+      <c r="C27" s="3">
+        <v>1650</v>
+      </c>
+      <c r="D27" s="3">
+        <f>E27/0.0393701/1000</f>
+        <v>41.909977368612218</v>
+      </c>
+      <c r="E27" s="3">
+        <v>1650</v>
+      </c>
+      <c r="F27" s="3">
+        <f>G27/0.0393701/1000</f>
+        <v>33.019982169209634</v>
+      </c>
+      <c r="G27" s="3">
+        <v>1300</v>
+      </c>
+      <c r="H27" s="3">
+        <f>I27/0.0393701/1000</f>
+        <v>29.209984226608519</v>
+      </c>
+      <c r="I27" s="3">
+        <v>1150</v>
+      </c>
+      <c r="J27" s="3">
+        <v>1150</v>
+      </c>
+      <c r="K27" s="3">
         <v>0</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="K18" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="L18" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="M18" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B19">
-        <f>C19/0.0393701/1000</f>
-        <v>47.62497428251389</v>
-      </c>
-      <c r="C19">
-        <v>1875</v>
-      </c>
-      <c r="D19">
-        <f>E19/0.0393701/1000</f>
-        <v>73.024960566521301</v>
-      </c>
-      <c r="E19">
-        <v>2875</v>
-      </c>
-      <c r="F19">
-        <f>G19/0.0393701/1000</f>
-        <v>33.019982169209634</v>
-      </c>
-      <c r="G19">
-        <v>1300</v>
-      </c>
-      <c r="H19">
-        <f>I19/0.0393701/1000</f>
-        <v>29.209984226608519</v>
-      </c>
-      <c r="I19">
-        <v>1150</v>
-      </c>
-      <c r="J19">
-        <v>1150</v>
-      </c>
-      <c r="K19">
+      <c r="L27" s="3">
+        <f>M27/0.0393701/1000</f>
         <v>0</v>
       </c>
-      <c r="L19">
-        <f>M19/0.0393701/1000</f>
+      <c r="M27" s="3">
         <v>0</v>
       </c>
-      <c r="M19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="N27" s="1">
+        <f>G27/B9</f>
+        <v>0.55741652490945692</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B20">
-        <f t="shared" ref="B20:D21" si="5">C20/0.0393701/1000</f>
+      <c r="B28" s="3">
+        <f t="shared" ref="B28:D29" si="5">C28/0.0393701/1000</f>
         <v>46.989974625413709</v>
       </c>
-      <c r="C20">
+      <c r="C28" s="3">
         <v>1850</v>
       </c>
-      <c r="D20">
+      <c r="D28" s="3">
         <f t="shared" si="5"/>
         <v>46.989974625413709</v>
       </c>
-      <c r="E20">
+      <c r="E28" s="3">
         <v>1850</v>
       </c>
-      <c r="F20">
-        <f t="shared" ref="F20" si="6">G20/0.0393701/1000</f>
+      <c r="F28" s="3">
+        <f t="shared" ref="F28" si="6">G28/0.0393701/1000</f>
         <v>38.09997942601111</v>
       </c>
-      <c r="G20">
+      <c r="G28" s="3">
         <v>1500</v>
       </c>
-      <c r="H20">
-        <f t="shared" ref="H20:J20" si="7">I20/0.0393701/1000</f>
+      <c r="H28" s="3">
+        <f t="shared" ref="H28:J28" si="7">I28/0.0393701/1000</f>
         <v>2.539998628400741</v>
       </c>
-      <c r="I20">
+      <c r="I28" s="3">
         <v>100</v>
       </c>
-      <c r="J20">
+      <c r="J28" s="3">
         <f t="shared" si="7"/>
         <v>12.699993142003704</v>
       </c>
-      <c r="K20">
+      <c r="K28" s="3">
         <v>500</v>
       </c>
-      <c r="L20">
-        <f t="shared" ref="L20" si="8">M20/0.0393701/1000</f>
+      <c r="L28" s="3">
+        <f t="shared" ref="L28" si="8">M28/0.0393701/1000</f>
         <v>0</v>
       </c>
-      <c r="M20">
+      <c r="M28" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="N28" s="1">
+        <f>G28/B9</f>
+        <v>0.64317291335706572</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B21">
+      <c r="B29" s="3">
         <f t="shared" si="5"/>
         <v>4.8259973939614072E-2</v>
       </c>
-      <c r="C21">
+      <c r="C29" s="3">
         <v>1.9</v>
       </c>
-      <c r="D21">
+      <c r="D29" s="3">
         <f t="shared" si="5"/>
         <v>1.4477992181884223</v>
       </c>
-      <c r="E21">
+      <c r="E29" s="3">
         <v>57</v>
       </c>
-      <c r="F21">
-        <f t="shared" ref="F21" si="9">G21/0.0393701/1000</f>
+      <c r="F29" s="3">
+        <f t="shared" ref="F29" si="9">G29/0.0393701/1000</f>
         <v>4.8259973939614072E-2</v>
       </c>
-      <c r="G21">
+      <c r="G29" s="3">
         <v>1.9</v>
       </c>
-      <c r="H21">
-        <f t="shared" ref="H21:J21" si="10">I21/0.0393701/1000</f>
+      <c r="H29" s="3">
+        <f t="shared" ref="H29:J29" si="10">I29/0.0393701/1000</f>
         <v>4.8259973939614072E-2</v>
       </c>
-      <c r="I21">
+      <c r="I29" s="3">
         <v>1.9</v>
       </c>
-      <c r="J21">
+      <c r="J29" s="3">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="K21">
+      <c r="K29" s="3">
         <v>0</v>
       </c>
-      <c r="L21">
-        <f t="shared" ref="L21" si="11">M21/0.0393701/1000</f>
+      <c r="L29" s="3">
+        <f t="shared" ref="L29" si="11">M29/0.0393701/1000</f>
         <v>0</v>
       </c>
-      <c r="M21">
+      <c r="M29" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B31" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C32" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C23" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
-        <v>34</v>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C33" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B11" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add new revision for patch antenna
New revision shrinks the first revision patch antenna dimensions to
achieve a higher resonance frequency. Feedline was moved closer to the
center to lower the characteristic impedance. The SMA footprint was
edited to remove error with unconnected thermal relief. Layout for the
antenna was simplified with the footprint creator.
</commit_message>
<xml_diff>
--- a/specs/patch_antenna-calculations.xlsx
+++ b/specs/patch_antenna-calculations.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeffrey Zheng\Dropbox\HA-HA\specs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jzheng13\Documents\HA-HA\specs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="42">
   <si>
     <t>Ground (mm)</t>
   </si>
@@ -101,9 +101,6 @@
     <t>+/-0.2</t>
   </si>
   <si>
-    <t>Actual Design</t>
-  </si>
-  <si>
     <t>Feed Pos X (mm)</t>
   </si>
   <si>
@@ -138,6 +135,21 @@
   </si>
   <si>
     <t>Effecitve dielectric constant of reference design is 3.86.</t>
+  </si>
+  <si>
+    <t>Actual Design r0.1</t>
+  </si>
+  <si>
+    <t>Actual Design r0.2</t>
+  </si>
+  <si>
+    <t>Feed line should have the full width going into the signal net as opposed to a thin thermal relief.</t>
+  </si>
+  <si>
+    <t>Actual Design Notes r0.1</t>
+  </si>
+  <si>
+    <t>Resonance at about 2.2GHz and 90ohm impedance.</t>
   </si>
 </sst>
 </file>
@@ -540,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O33"/>
+  <dimension ref="A1:O43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,10 +605,10 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" s="3">
-        <f>(B3+1)/2+(B3-1)/2*((SQRT(1+12*B6/G14))^-1)</f>
+        <f>($B$3+1)/2+($B$3-1)/2*((SQRT(1+12*$B$6/$G$14))^-1)</f>
         <v>4.2728372472104468</v>
       </c>
     </row>
@@ -632,7 +644,7 @@
         <v>21</v>
       </c>
       <c r="B8" s="3">
-        <f>300000000/(B7*10^6)/SQRT(B4)</f>
+        <f>300000000/($B$7*10^6)/SQRT($B$4)</f>
         <v>59.237537269949385</v>
       </c>
     </row>
@@ -641,15 +653,15 @@
         <v>22</v>
       </c>
       <c r="B9" s="3">
-        <f>B8*0.0393701*1000</f>
+        <f>$B$8*0.0393701*1000</f>
         <v>2332.1877660716345</v>
       </c>
       <c r="C9" s="3">
-        <f>B9/2</f>
+        <f>$B$9/2</f>
         <v>1166.0938830358173</v>
       </c>
       <c r="D9" s="3">
-        <f>B9/4</f>
+        <f>$B$9/4</f>
         <v>583.04694151790864</v>
       </c>
     </row>
@@ -661,7 +673,7 @@
         <v>18</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -723,11 +735,11 @@
         <v>511.81129999999996</v>
       </c>
       <c r="J13" s="1">
-        <f>G13/B9</f>
+        <f>G13/$B$9</f>
         <v>0.55707920215549822</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -763,11 +775,11 @@
         <v>118.1103</v>
       </c>
       <c r="J14" s="1">
-        <f>G14/B9</f>
+        <f>G14/$B$9</f>
         <v>0.64148514187602823</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -806,10 +818,10 @@
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
@@ -832,7 +844,7 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -861,16 +873,16 @@
         <v>7</v>
       </c>
       <c r="J26" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M26" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M26" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
@@ -919,11 +931,11 @@
         <v>0</v>
       </c>
       <c r="N27" s="1">
-        <f>G27/B9</f>
+        <f>G27/$B$9</f>
         <v>0.55741652490945692</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
@@ -973,11 +985,11 @@
         <v>0</v>
       </c>
       <c r="N28" s="1">
-        <f>G28/B9</f>
+        <f>G28/$B$9</f>
         <v>0.64317291335706572</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
@@ -1029,20 +1041,236 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C32" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C33" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B34" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M37" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B38" s="3">
+        <f>C38/0.0393701/1000</f>
+        <v>38.734979083111298</v>
+      </c>
+      <c r="C38" s="3">
+        <v>1525</v>
+      </c>
+      <c r="D38" s="3">
+        <f>E38/0.0393701/1000</f>
+        <v>38.734979083111298</v>
+      </c>
+      <c r="E38" s="3">
+        <v>1525</v>
+      </c>
+      <c r="F38" s="3">
+        <f>G38/0.0393701/1000</f>
+        <v>30.479983540808892</v>
+      </c>
+      <c r="G38" s="3">
+        <v>1200</v>
+      </c>
+      <c r="H38" s="3">
+        <f>I38/0.0393701/1000</f>
+        <v>29.209984226608519</v>
+      </c>
+      <c r="I38" s="3">
+        <v>1150</v>
+      </c>
+      <c r="J38" s="3">
+        <v>1150</v>
+      </c>
+      <c r="K38" s="3">
+        <v>0</v>
+      </c>
+      <c r="L38" s="3">
+        <f>M38/0.0393701/1000</f>
+        <v>0</v>
+      </c>
+      <c r="M38" s="3">
+        <v>0</v>
+      </c>
+      <c r="N38" s="1">
+        <f>G38/$B$9</f>
+        <v>0.51453833068565258</v>
+      </c>
+      <c r="O38" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39" s="3">
+        <f t="shared" ref="B39:B40" si="12">C39/0.0393701/1000</f>
+        <v>43.179976682812594</v>
+      </c>
+      <c r="C39" s="3">
+        <v>1700</v>
+      </c>
+      <c r="D39" s="3">
+        <f t="shared" ref="D39:D40" si="13">E39/0.0393701/1000</f>
+        <v>43.179976682812594</v>
+      </c>
+      <c r="E39" s="3">
+        <v>1700</v>
+      </c>
+      <c r="F39" s="3">
+        <f t="shared" ref="F39:F40" si="14">G39/0.0393701/1000</f>
+        <v>34.924981140510184</v>
+      </c>
+      <c r="G39" s="3">
+        <v>1375</v>
+      </c>
+      <c r="H39" s="3">
+        <f t="shared" ref="H39:H40" si="15">I39/0.0393701/1000</f>
+        <v>2.539998628400741</v>
+      </c>
+      <c r="I39" s="3">
+        <v>100</v>
+      </c>
+      <c r="J39" s="3">
+        <f t="shared" ref="J39:J40" si="16">K39/0.0393701/1000</f>
+        <v>12.699993142003704</v>
+      </c>
+      <c r="K39" s="3">
+        <v>500</v>
+      </c>
+      <c r="L39" s="3">
+        <f t="shared" ref="L39:L40" si="17">M39/0.0393701/1000</f>
+        <v>0</v>
+      </c>
+      <c r="M39" s="3">
+        <v>0</v>
+      </c>
+      <c r="N39" s="1">
+        <f>G39/$B$9</f>
+        <v>0.58957517057731024</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40" s="3">
+        <f t="shared" si="12"/>
+        <v>4.8259973939614072E-2</v>
+      </c>
+      <c r="C40" s="3">
+        <v>1.9</v>
+      </c>
+      <c r="D40" s="3">
+        <f t="shared" si="13"/>
+        <v>1.4477992181884223</v>
+      </c>
+      <c r="E40" s="3">
+        <v>57</v>
+      </c>
+      <c r="F40" s="3">
+        <f t="shared" si="14"/>
+        <v>4.8259973939614072E-2</v>
+      </c>
+      <c r="G40" s="3">
+        <v>1.9</v>
+      </c>
+      <c r="H40" s="3">
+        <f t="shared" si="15"/>
+        <v>4.8259973939614072E-2</v>
+      </c>
+      <c r="I40" s="3">
+        <v>1.9</v>
+      </c>
+      <c r="J40" s="3">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="K40" s="3">
+        <v>0</v>
+      </c>
+      <c r="L40" s="3">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="M40" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B42" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C43" s="3" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new tests for patch antenna
Two new test boards laid out to test impedance and performance due to
the effect of larger copper void space in the presence of nearby ground
copper, one board with a matching circuit and the other without. Traces
no longer follow the optimal transmission line width for 50ohm
performance due to the use of 0402 SMD technology.
</commit_message>
<xml_diff>
--- a/specs/patch_antenna-calculations.xlsx
+++ b/specs/patch_antenna-calculations.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jzheng13\Documents\HA-HA\specs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeffrey Zheng\Dropbox\HA-HA\specs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="43">
   <si>
     <t>Ground (mm)</t>
   </si>
@@ -150,6 +150,9 @@
   </si>
   <si>
     <t>Resonance at about 2.2GHz and 90ohm impedance.</t>
+  </si>
+  <si>
+    <t>Top copper void increased to avoid fringe field interference with larger circuit layout.</t>
   </si>
 </sst>
 </file>
@@ -552,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O43"/>
+  <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -918,7 +921,8 @@
         <v>1150</v>
       </c>
       <c r="J27" s="3">
-        <v>1150</v>
+        <f t="shared" ref="H27:J28" si="5">K27/0.0393701/1000</f>
+        <v>0</v>
       </c>
       <c r="K27" s="3">
         <v>0</v>
@@ -943,35 +947,35 @@
         <v>8</v>
       </c>
       <c r="B28" s="3">
-        <f t="shared" ref="B28:D29" si="5">C28/0.0393701/1000</f>
+        <f t="shared" ref="B28:D29" si="6">C28/0.0393701/1000</f>
         <v>46.989974625413709</v>
       </c>
       <c r="C28" s="3">
         <v>1850</v>
       </c>
       <c r="D28" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>46.989974625413709</v>
       </c>
       <c r="E28" s="3">
         <v>1850</v>
       </c>
       <c r="F28" s="3">
-        <f t="shared" ref="F28" si="6">G28/0.0393701/1000</f>
+        <f t="shared" ref="F28" si="7">G28/0.0393701/1000</f>
         <v>38.09997942601111</v>
       </c>
       <c r="G28" s="3">
         <v>1500</v>
       </c>
       <c r="H28" s="3">
-        <f t="shared" ref="H28:J28" si="7">I28/0.0393701/1000</f>
+        <f t="shared" si="5"/>
         <v>2.539998628400741</v>
       </c>
       <c r="I28" s="3">
         <v>100</v>
       </c>
       <c r="J28" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>12.699993142003704</v>
       </c>
       <c r="K28" s="3">
@@ -997,14 +1001,14 @@
         <v>10</v>
       </c>
       <c r="B29" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.8259973939614072E-2</v>
       </c>
       <c r="C29" s="3">
         <v>1.9</v>
       </c>
       <c r="D29" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.4477992181884223</v>
       </c>
       <c r="E29" s="3">
@@ -1105,9 +1109,6 @@
         <v>26</v>
       </c>
       <c r="N37" s="1"/>
-      <c r="O37" s="1" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
@@ -1115,17 +1116,17 @@
       </c>
       <c r="B38" s="3">
         <f>C38/0.0393701/1000</f>
-        <v>38.734979083111298</v>
+        <v>45.719975311213332</v>
       </c>
       <c r="C38" s="3">
-        <v>1525</v>
+        <v>1800</v>
       </c>
       <c r="D38" s="3">
         <f>E38/0.0393701/1000</f>
-        <v>38.734979083111298</v>
+        <v>45.719975311213332</v>
       </c>
       <c r="E38" s="3">
-        <v>1525</v>
+        <v>1800</v>
       </c>
       <c r="F38" s="3">
         <f>G38/0.0393701/1000</f>
@@ -1136,13 +1137,14 @@
       </c>
       <c r="H38" s="3">
         <f>I38/0.0393701/1000</f>
-        <v>29.209984226608519</v>
+        <v>15.239991770404446</v>
       </c>
       <c r="I38" s="3">
-        <v>1150</v>
+        <v>600</v>
       </c>
       <c r="J38" s="3">
-        <v>1150</v>
+        <f t="shared" ref="J38:J40" si="12">K38/0.0393701/1000</f>
+        <v>0</v>
       </c>
       <c r="K38" s="3">
         <v>0</v>
@@ -1167,39 +1169,39 @@
         <v>8</v>
       </c>
       <c r="B39" s="3">
-        <f t="shared" ref="B39:B40" si="12">C39/0.0393701/1000</f>
-        <v>43.179976682812594</v>
+        <f t="shared" ref="B39:B40" si="13">C39/0.0393701/1000</f>
+        <v>50.799972568014816</v>
       </c>
       <c r="C39" s="3">
-        <v>1700</v>
+        <v>2000</v>
       </c>
       <c r="D39" s="3">
-        <f t="shared" ref="D39:D40" si="13">E39/0.0393701/1000</f>
-        <v>43.179976682812594</v>
+        <f t="shared" ref="D39:D40" si="14">E39/0.0393701/1000</f>
+        <v>50.799972568014816</v>
       </c>
       <c r="E39" s="3">
-        <v>1700</v>
+        <v>2000</v>
       </c>
       <c r="F39" s="3">
-        <f t="shared" ref="F39:F40" si="14">G39/0.0393701/1000</f>
+        <f t="shared" ref="F39:F40" si="15">G39/0.0393701/1000</f>
         <v>34.924981140510184</v>
       </c>
       <c r="G39" s="3">
         <v>1375</v>
       </c>
       <c r="H39" s="3">
-        <f t="shared" ref="H39:H40" si="15">I39/0.0393701/1000</f>
-        <v>2.539998628400741</v>
+        <f t="shared" ref="H39:H40" si="16">I39/0.0393701/1000</f>
+        <v>0.50799972568014817</v>
       </c>
       <c r="I39" s="3">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="J39" s="3">
-        <f t="shared" ref="J39:J40" si="16">K39/0.0393701/1000</f>
-        <v>12.699993142003704</v>
+        <f t="shared" si="12"/>
+        <v>13.969992456204075</v>
       </c>
       <c r="K39" s="3">
-        <v>500</v>
+        <v>550</v>
       </c>
       <c r="L39" s="3">
         <f t="shared" ref="L39:L40" si="17">M39/0.0393701/1000</f>
@@ -1212,41 +1214,44 @@
         <f>G39/$B$9</f>
         <v>0.58957517057731024</v>
       </c>
+      <c r="O39" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B40" s="3">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>4.8259973939614072E-2</v>
       </c>
       <c r="C40" s="3">
         <v>1.9</v>
       </c>
       <c r="D40" s="3">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1.4477992181884223</v>
       </c>
       <c r="E40" s="3">
         <v>57</v>
       </c>
       <c r="F40" s="3">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>4.8259973939614072E-2</v>
       </c>
       <c r="G40" s="3">
         <v>1.9</v>
       </c>
       <c r="H40" s="3">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>4.8259973939614072E-2</v>
       </c>
       <c r="I40" s="3">
         <v>1.9</v>
       </c>
       <c r="J40" s="3">
-        <f t="shared" si="16"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="K40" s="3">
@@ -1271,6 +1276,11 @@
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C43" s="3" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C44" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>